<commit_message>
Fixed closing predict#.csv files
And added method to obtain N rows with largest values
</commit_message>
<xml_diff>
--- a/Assignment 2/Progress Report Nick.xlsx
+++ b/Assignment 2/Progress Report Nick.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="5" documentId="6_{9612CC59-CCF8-4019-98D4-5C9C24381B54}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{B162788D-1498-4CAF-BDB1-2C9EE5F5E673}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="6_{9612CC59-CCF8-4019-98D4-5C9C24381B54}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{2FC241CC-02A2-4933-8D82-98907BA2708A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Start</t>
   </si>
@@ -49,6 +49,9 @@
     <t>Implemented averages over srch_id for some columns and difference between this average per row. 
 Also performed 10-fold cross-validation on the complete dataset (which took more than an hour) and 
 obtained a score of 0.540 +/- 0.003!</t>
+  </si>
+  <si>
+    <t>Discussed planning, things to do with team</t>
   </si>
 </sst>
 </file>
@@ -370,19 +373,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="96.140625" customWidth="1"/>
+    <col min="1" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="96.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -393,7 +396,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43218.708333333336</v>
       </c>
@@ -404,7 +407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43222.770833333336</v>
       </c>
@@ -415,7 +418,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>43223.541666666664</v>
       </c>
@@ -426,7 +429,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>43225.666666666664</v>
       </c>
@@ -437,7 +440,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>43226.75</v>
       </c>
@@ -448,7 +451,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>43228.802083333336</v>
       </c>
@@ -457,6 +460,17 @@
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>43234.59375</v>
+      </c>
+      <c r="B8" s="1">
+        <v>43234.645833333336</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added prediction section for test_set
</commit_message>
<xml_diff>
--- a/Assignment 2/Progress Report Nick.xlsx
+++ b/Assignment 2/Progress Report Nick.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="30" documentId="6_{9612CC59-CCF8-4019-98D4-5C9C24381B54}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{16CA01B2-0AD5-4D22-93D0-BFAC3180BC50}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="6_{9612CC59-CCF8-4019-98D4-5C9C24381B54}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{6D32FB45-8DFB-4B04-A833-0FE8D54833B3}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Start</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Fixed NDCG-implementation to use Kaggle's method. Score has decreased to 0.477 +/- 0.002</t>
+  </si>
+  <si>
+    <t>Create code to generate final_predict.csv containing ordering in test_set</t>
   </si>
 </sst>
 </file>
@@ -385,19 +388,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="96.109375" customWidth="1"/>
+    <col min="1" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="96.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,7 +411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43218.708333333336</v>
       </c>
@@ -419,7 +422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43222.770833333336</v>
       </c>
@@ -430,7 +433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43223.541666666664</v>
       </c>
@@ -441,7 +444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43225.666666666664</v>
       </c>
@@ -452,7 +455,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43226.75</v>
       </c>
@@ -463,7 +466,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43228.802083333336</v>
       </c>
@@ -474,7 +477,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43234.59375</v>
       </c>
@@ -485,7 +488,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43234.822916666664</v>
       </c>
@@ -496,7 +499,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43236.802083333336</v>
       </c>
@@ -507,7 +510,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43240.395833333336</v>
       </c>
@@ -518,7 +521,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43242.458333333336</v>
       </c>
@@ -527,6 +530,17 @@
       </c>
       <c r="C12" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43246.666666666664</v>
+      </c>
+      <c r="B13" s="1">
+        <v>43246.75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Further commented the code and included final_predict.csv in a zip-file
</commit_message>
<xml_diff>
--- a/Assignment 2/Progress Report Nick.xlsx
+++ b/Assignment 2/Progress Report Nick.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="33" documentId="6_{9612CC59-CCF8-4019-98D4-5C9C24381B54}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{6D32FB45-8DFB-4B04-A833-0FE8D54833B3}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="6_{9612CC59-CCF8-4019-98D4-5C9C24381B54}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{8D75CDF4-9656-469A-A199-30B793A3C313}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Start</t>
   </si>
@@ -67,6 +67,11 @@
   </si>
   <si>
     <t>Create code to generate final_predict.csv containing ordering in test_set</t>
+  </si>
+  <si>
+    <t>Tested final_predict.csv using the Kaggle-version of the datasets. 
+Obtained a private score of 0.48391 and public score of 0.48574. 
+Also further commented the code</t>
   </si>
 </sst>
 </file>
@@ -388,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,6 +548,14 @@
         <v>14</v>
       </c>
     </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>43246.770833333336</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>